<commit_message>
added hyp param tune
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>eval_avg_ep_rew</t>
-  </si>
-  <si>
-    <t>eval_max_ep_rew</t>
-  </si>
-  <si>
-    <t>eval_min_ep_rew</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>total_time_taken(m)</t>
   </si>
   <si>
     <t>eval_ach_goal_perc</t>
@@ -128,6 +122,9 @@
   </si>
   <si>
     <t>A_critic_agg_weight</t>
+  </si>
+  <si>
+    <t>O_num_agents</t>
   </si>
   <si>
     <t>O_reach_goal_rew</t>
@@ -491,13 +488,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,8 +612,457 @@
       <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
+    </row>
+    <row r="2" spans="1:39">
+      <c r="A2">
+        <v>0.6579903721809387</v>
+      </c>
+      <c r="B2">
+        <v>0.303030303030303</v>
+      </c>
+      <c r="C2">
+        <v>3.41</v>
+      </c>
+      <c r="D2">
+        <v>9.24</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>128</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>202</v>
+      </c>
+      <c r="Q2">
+        <v>42</v>
+      </c>
+      <c r="S2">
+        <v>32</v>
+      </c>
+      <c r="U2">
+        <v>32</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>32</v>
+      </c>
+      <c r="Z2">
+        <v>0.95</v>
+      </c>
+      <c r="AA2">
+        <v>0.01</v>
+      </c>
+      <c r="AB2">
+        <v>32</v>
+      </c>
+      <c r="AC2">
+        <v>10</v>
+      </c>
+      <c r="AD2">
+        <v>0.2</v>
+      </c>
+      <c r="AE2">
+        <v>0.9</v>
+      </c>
+      <c r="AF2">
+        <v>0.001</v>
+      </c>
+      <c r="AG2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>5</v>
+      </c>
+      <c r="AI2">
+        <v>0.8</v>
+      </c>
+      <c r="AJ2">
+        <v>0.9</v>
+      </c>
+      <c r="AK2">
+        <v>8</v>
+      </c>
+      <c r="AL2">
+        <v>10</v>
+      </c>
+      <c r="AM2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
+      <c r="A3">
+        <v>0.603220264116923</v>
+      </c>
+      <c r="B3">
+        <v>0.2626262626262627</v>
+      </c>
+      <c r="C3">
+        <v>3.37</v>
+      </c>
+      <c r="D3">
+        <v>9.15</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>128</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>202</v>
+      </c>
+      <c r="Q3">
+        <v>42</v>
+      </c>
+      <c r="S3">
+        <v>32</v>
+      </c>
+      <c r="U3">
+        <v>32</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>32</v>
+      </c>
+      <c r="Z3">
+        <v>0.95</v>
+      </c>
+      <c r="AA3">
+        <v>0.01</v>
+      </c>
+      <c r="AB3">
+        <v>32</v>
+      </c>
+      <c r="AC3">
+        <v>10</v>
+      </c>
+      <c r="AD3">
+        <v>0.2</v>
+      </c>
+      <c r="AE3">
+        <v>0.9</v>
+      </c>
+      <c r="AF3">
+        <v>0.001</v>
+      </c>
+      <c r="AG3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>5</v>
+      </c>
+      <c r="AI3">
+        <v>0.8</v>
+      </c>
+      <c r="AJ3">
+        <v>0.9</v>
+      </c>
+      <c r="AK3">
+        <v>8</v>
+      </c>
+      <c r="AL3">
+        <v>10</v>
+      </c>
+      <c r="AM3">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
+      <c r="A4">
+        <v>0.5995295246442159</v>
+      </c>
+      <c r="B4">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="C4">
+        <v>3.35</v>
+      </c>
+      <c r="D4">
+        <v>8.98</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>128</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>40</v>
+      </c>
+      <c r="P4">
+        <v>202</v>
+      </c>
+      <c r="Q4">
+        <v>42</v>
+      </c>
+      <c r="S4">
+        <v>32</v>
+      </c>
+      <c r="U4">
+        <v>32</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>32</v>
+      </c>
+      <c r="Z4">
+        <v>0.95</v>
+      </c>
+      <c r="AA4">
+        <v>0.01</v>
+      </c>
+      <c r="AB4">
+        <v>32</v>
+      </c>
+      <c r="AC4">
+        <v>10</v>
+      </c>
+      <c r="AD4">
+        <v>0.2</v>
+      </c>
+      <c r="AE4">
+        <v>0.95</v>
+      </c>
+      <c r="AF4">
+        <v>0.001</v>
+      </c>
+      <c r="AG4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>5</v>
+      </c>
+      <c r="AI4">
+        <v>0.2</v>
+      </c>
+      <c r="AJ4">
+        <v>0.75</v>
+      </c>
+      <c r="AK4">
+        <v>8</v>
+      </c>
+      <c r="AL4">
+        <v>10</v>
+      </c>
+      <c r="AM4">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
+      <c r="A5">
+        <v>0.5993634541829427</v>
+      </c>
+      <c r="B5">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="C5">
+        <v>3.48</v>
+      </c>
+      <c r="D5">
+        <v>8.82</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>128</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>40</v>
+      </c>
+      <c r="P5">
+        <v>202</v>
+      </c>
+      <c r="Q5">
+        <v>42</v>
+      </c>
+      <c r="S5">
+        <v>32</v>
+      </c>
+      <c r="U5">
+        <v>32</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>32</v>
+      </c>
+      <c r="Z5">
+        <v>0.95</v>
+      </c>
+      <c r="AA5">
+        <v>0.01</v>
+      </c>
+      <c r="AB5">
+        <v>32</v>
+      </c>
+      <c r="AC5">
+        <v>10</v>
+      </c>
+      <c r="AD5">
+        <v>0.2</v>
+      </c>
+      <c r="AE5">
+        <v>0.95</v>
+      </c>
+      <c r="AF5">
+        <v>0.001</v>
+      </c>
+      <c r="AG5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>5</v>
+      </c>
+      <c r="AI5">
+        <v>0.2</v>
+      </c>
+      <c r="AJ5">
+        <v>0.75</v>
+      </c>
+      <c r="AK5">
+        <v>8</v>
+      </c>
+      <c r="AL5">
+        <v>10</v>
+      </c>
+      <c r="AM5">
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added back toy data
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -151,7 +151,7 @@
     <t>no_structure</t>
   </si>
   <si>
-    <t>very hard</t>
+    <t>very easy</t>
   </si>
 </sst>
 </file>
@@ -642,16 +642,16 @@
     </row>
     <row r="2" spans="1:41">
       <c r="A2">
-        <v>31.52176719506582</v>
+        <v>31.22534311612447</v>
       </c>
       <c r="B2">
-        <v>0.4242424242424243</v>
+        <v>0.2828282828282828</v>
       </c>
       <c r="C2">
-        <v>3.69</v>
+        <v>3.89</v>
       </c>
       <c r="D2">
-        <v>13.39</v>
+        <v>17.38</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -684,16 +684,16 @@
         <v>41</v>
       </c>
       <c r="O2">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P2">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q2">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R2">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -767,16 +767,16 @@
     </row>
     <row r="3" spans="1:41">
       <c r="A3">
-        <v>28.10683162212372</v>
+        <v>31.61318896214167</v>
       </c>
       <c r="B3">
-        <v>0.3535353535353535</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="C3">
-        <v>3.68</v>
+        <v>3.91</v>
       </c>
       <c r="D3">
-        <v>15.8</v>
+        <v>16.56</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -809,16 +809,16 @@
         <v>41</v>
       </c>
       <c r="O3">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P3">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q3">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R3">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S3">
         <v>32</v>
@@ -892,16 +892,16 @@
     </row>
     <row r="4" spans="1:41">
       <c r="A4">
-        <v>29.55733622312546</v>
+        <v>33.53106116453807</v>
       </c>
       <c r="B4">
-        <v>0.4343434343434344</v>
+        <v>0.3131313131313131</v>
       </c>
       <c r="C4">
-        <v>3.82</v>
+        <v>3.68</v>
       </c>
       <c r="D4">
-        <v>13.32</v>
+        <v>15.72</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -934,16 +934,16 @@
         <v>41</v>
       </c>
       <c r="O4">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P4">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q4">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R4">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S4">
         <v>32</v>
@@ -1017,16 +1017,16 @@
     </row>
     <row r="5" spans="1:41">
       <c r="A5">
-        <v>20.5165269056956</v>
+        <v>20.50241411526998</v>
       </c>
       <c r="B5">
-        <v>0.5050505050505051</v>
+        <v>0.202020202020202</v>
       </c>
       <c r="C5">
-        <v>3.89</v>
+        <v>3.95</v>
       </c>
       <c r="D5">
-        <v>12.85</v>
+        <v>18.25</v>
       </c>
       <c r="E5">
         <v>1000</v>
@@ -1059,16 +1059,16 @@
         <v>42</v>
       </c>
       <c r="O5">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P5">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q5">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R5">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S5">
         <v>32</v>
@@ -1142,16 +1142,16 @@
     </row>
     <row r="6" spans="1:41">
       <c r="A6">
-        <v>20.74681055148443</v>
+        <v>20.97510018348694</v>
       </c>
       <c r="B6">
-        <v>0.4545454545454545</v>
+        <v>0.2626262626262627</v>
       </c>
       <c r="C6">
-        <v>3.76</v>
+        <v>3.79</v>
       </c>
       <c r="D6">
-        <v>13.27</v>
+        <v>17.72</v>
       </c>
       <c r="E6">
         <v>1000</v>
@@ -1184,16 +1184,16 @@
         <v>42</v>
       </c>
       <c r="O6">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P6">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q6">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R6">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S6">
         <v>32</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="7" spans="1:41">
       <c r="A7">
-        <v>20.45671214660009</v>
+        <v>21.01098755598068</v>
       </c>
       <c r="B7">
-        <v>0.5151515151515151</v>
+        <v>0.2323232323232323</v>
       </c>
       <c r="C7">
-        <v>3.72</v>
+        <v>3.85</v>
       </c>
       <c r="D7">
-        <v>12.8</v>
+        <v>17.21</v>
       </c>
       <c r="E7">
         <v>1000</v>
@@ -1309,16 +1309,16 @@
         <v>42</v>
       </c>
       <c r="O7">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P7">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q7">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R7">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S7">
         <v>32</v>
@@ -1392,16 +1392,16 @@
     </row>
     <row r="8" spans="1:41">
       <c r="A8">
-        <v>10.74654963413874</v>
+        <v>11.10944559176763</v>
       </c>
       <c r="B8">
-        <v>0.4545454545454545</v>
+        <v>0.2626262626262627</v>
       </c>
       <c r="C8">
-        <v>3.72</v>
+        <v>3.87</v>
       </c>
       <c r="D8">
-        <v>13.69</v>
+        <v>16.46</v>
       </c>
       <c r="E8">
         <v>1000</v>
@@ -1434,16 +1434,16 @@
         <v>43</v>
       </c>
       <c r="O8">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P8">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q8">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R8">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S8">
         <v>32</v>
@@ -1517,16 +1517,16 @@
     </row>
     <row r="9" spans="1:41">
       <c r="A9">
-        <v>11.09661258459091</v>
+        <v>11.95082873503367</v>
       </c>
       <c r="B9">
-        <v>0.5555555555555556</v>
+        <v>0.3434343434343434</v>
       </c>
       <c r="C9">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="D9">
-        <v>12.42</v>
+        <v>15.49</v>
       </c>
       <c r="E9">
         <v>1000</v>
@@ -1559,16 +1559,16 @@
         <v>43</v>
       </c>
       <c r="O9">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P9">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q9">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R9">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S9">
         <v>32</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="10" spans="1:41">
       <c r="A10">
-        <v>10.89122907320658</v>
+        <v>11.89163700342178</v>
       </c>
       <c r="B10">
-        <v>0.5252525252525253</v>
+        <v>0.4141414141414141</v>
       </c>
       <c r="C10">
-        <v>3.91</v>
+        <v>3.75</v>
       </c>
       <c r="D10">
-        <v>13.33</v>
+        <v>14.42</v>
       </c>
       <c r="E10">
         <v>1000</v>
@@ -1684,16 +1684,16 @@
         <v>43</v>
       </c>
       <c r="O10">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P10">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q10">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R10">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S10">
         <v>32</v>
@@ -1767,16 +1767,16 @@
     </row>
     <row r="11" spans="1:41">
       <c r="A11">
-        <v>8.22238165140152</v>
+        <v>8.372995054721832</v>
       </c>
       <c r="B11">
-        <v>0.5151515151515151</v>
+        <v>0.2424242424242424</v>
       </c>
       <c r="C11">
-        <v>3.68</v>
+        <v>3.82</v>
       </c>
       <c r="D11">
-        <v>12.98</v>
+        <v>16.87</v>
       </c>
       <c r="E11">
         <v>1000</v>
@@ -1809,16 +1809,16 @@
         <v>44</v>
       </c>
       <c r="O11">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P11">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q11">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R11">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S11">
         <v>32</v>
@@ -1892,16 +1892,16 @@
     </row>
     <row r="12" spans="1:41">
       <c r="A12">
-        <v>8.189760696887969</v>
+        <v>8.535145397981008</v>
       </c>
       <c r="B12">
-        <v>0.4747474747474748</v>
+        <v>0.1717171717171717</v>
       </c>
       <c r="C12">
-        <v>3.63</v>
+        <v>3.91</v>
       </c>
       <c r="D12">
-        <v>12.82</v>
+        <v>17.42</v>
       </c>
       <c r="E12">
         <v>1000</v>
@@ -1934,16 +1934,16 @@
         <v>44</v>
       </c>
       <c r="O12">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P12">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q12">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R12">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S12">
         <v>32</v>
@@ -2017,16 +2017,16 @@
     </row>
     <row r="13" spans="1:41">
       <c r="A13">
-        <v>8.071684153874715</v>
+        <v>8.086561504999796</v>
       </c>
       <c r="B13">
-        <v>0.3838383838383838</v>
+        <v>0.2323232323232323</v>
       </c>
       <c r="C13">
-        <v>3.64</v>
+        <v>3.79</v>
       </c>
       <c r="D13">
-        <v>14.28</v>
+        <v>16.81</v>
       </c>
       <c r="E13">
         <v>1000</v>
@@ -2059,16 +2059,16 @@
         <v>44</v>
       </c>
       <c r="O13">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="P13">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="Q13">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="R13">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="S13">
         <v>32</v>

</xml_diff>

<commit_message>
added combined actor critic option
</commit_message>
<xml_diff>
--- a/run-data.xlsx
+++ b/run-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
   <si>
     <t>total_time_taken(m)</t>
   </si>
@@ -124,6 +124,9 @@
     <t>A_critic_agg_weight</t>
   </si>
   <si>
+    <t>A_combined_actor_critic</t>
+  </si>
+  <si>
     <t>O_num_agents</t>
   </si>
   <si>
@@ -139,19 +142,10 @@
     <t>O_data</t>
   </si>
   <si>
-    <t>deepmind</t>
-  </si>
-  <si>
     <t>nervenet</t>
   </si>
   <si>
-    <t>fully_connected</t>
-  </si>
-  <si>
-    <t>no_structure</t>
-  </si>
-  <si>
-    <t>very easy</t>
+    <t>toy2</t>
   </si>
 </sst>
 </file>
@@ -509,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO13"/>
+  <dimension ref="A1:AP34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,34 +633,37 @@
       <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:42">
       <c r="A2">
-        <v>31.22534311612447</v>
+        <v>9.770392139752706</v>
       </c>
       <c r="B2">
-        <v>0.2828282828282828</v>
+        <v>0.2525252525252525</v>
       </c>
       <c r="C2">
-        <v>3.89</v>
+        <v>3.52</v>
       </c>
       <c r="D2">
-        <v>17.38</v>
+        <v>6.97</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F2">
         <v>128</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -681,19 +678,19 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2">
         <v>41</v>
       </c>
-      <c r="O2">
-        <v>76</v>
-      </c>
       <c r="P2">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q2">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R2">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -749,49 +746,52 @@
       <c r="AJ2">
         <v>0.75</v>
       </c>
-      <c r="AK2">
-        <v>8</v>
+      <c r="AK2" t="b">
+        <v>0</v>
       </c>
       <c r="AL2">
+        <v>8</v>
+      </c>
+      <c r="AM2">
         <v>5</v>
       </c>
-      <c r="AM2">
-        <v>-5</v>
-      </c>
       <c r="AN2">
-        <v>1</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>45</v>
+        <v>-2</v>
+      </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:42">
       <c r="A3">
-        <v>31.61318896214167</v>
+        <v>9.542035957177481</v>
       </c>
       <c r="B3">
-        <v>0.2222222222222222</v>
+        <v>0.2828282828282828</v>
       </c>
       <c r="C3">
-        <v>3.91</v>
+        <v>3.55</v>
       </c>
       <c r="D3">
-        <v>16.56</v>
+        <v>7.06</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F3">
         <v>128</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -806,19 +806,19 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3">
         <v>41</v>
       </c>
-      <c r="O3">
-        <v>76</v>
-      </c>
       <c r="P3">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q3">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R3">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S3">
         <v>32</v>
@@ -874,49 +874,52 @@
       <c r="AJ3">
         <v>0.75</v>
       </c>
-      <c r="AK3">
-        <v>8</v>
+      <c r="AK3" t="b">
+        <v>0</v>
       </c>
       <c r="AL3">
+        <v>8</v>
+      </c>
+      <c r="AM3">
         <v>5</v>
       </c>
-      <c r="AM3">
-        <v>-5</v>
-      </c>
       <c r="AN3">
-        <v>1</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>45</v>
+        <v>-2</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:42">
       <c r="A4">
-        <v>33.53106116453807</v>
+        <v>9.385571563243866</v>
       </c>
       <c r="B4">
-        <v>0.3131313131313131</v>
+        <v>0.3535353535353535</v>
       </c>
       <c r="C4">
-        <v>3.68</v>
+        <v>3.67</v>
       </c>
       <c r="D4">
-        <v>15.72</v>
+        <v>6.76</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F4">
         <v>128</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -931,19 +934,19 @@
         <v>6</v>
       </c>
       <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4">
         <v>41</v>
       </c>
-      <c r="O4">
-        <v>76</v>
-      </c>
       <c r="P4">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q4">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R4">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S4">
         <v>32</v>
@@ -999,49 +1002,52 @@
       <c r="AJ4">
         <v>0.75</v>
       </c>
-      <c r="AK4">
-        <v>8</v>
+      <c r="AK4" t="b">
+        <v>0</v>
       </c>
       <c r="AL4">
+        <v>8</v>
+      </c>
+      <c r="AM4">
         <v>5</v>
       </c>
-      <c r="AM4">
-        <v>-5</v>
-      </c>
       <c r="AN4">
-        <v>1</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>45</v>
+        <v>-2</v>
+      </c>
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:42">
       <c r="A5">
-        <v>20.50241411526998</v>
+        <v>9.431532001495361</v>
       </c>
       <c r="B5">
-        <v>0.202020202020202</v>
+        <v>0.3838383838383838</v>
       </c>
       <c r="C5">
-        <v>3.95</v>
+        <v>3.66</v>
       </c>
       <c r="D5">
-        <v>18.25</v>
+        <v>6.88</v>
       </c>
       <c r="E5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F5">
         <v>128</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -1059,16 +1065,16 @@
         <v>42</v>
       </c>
       <c r="O5">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P5">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q5">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R5">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S5">
         <v>32</v>
@@ -1124,49 +1130,52 @@
       <c r="AJ5">
         <v>0.75</v>
       </c>
-      <c r="AK5">
-        <v>8</v>
+      <c r="AK5" t="b">
+        <v>0</v>
       </c>
       <c r="AL5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM5">
+        <v>10</v>
+      </c>
+      <c r="AN5">
         <v>-5</v>
       </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>45</v>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:42">
       <c r="A6">
-        <v>20.97510018348694</v>
+        <v>9.954400626818339</v>
       </c>
       <c r="B6">
-        <v>0.2626262626262627</v>
+        <v>0.3232323232323233</v>
       </c>
       <c r="C6">
-        <v>3.79</v>
+        <v>3.61</v>
       </c>
       <c r="D6">
-        <v>17.72</v>
+        <v>6.87</v>
       </c>
       <c r="E6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>128</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
       <c r="I6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -1184,16 +1193,16 @@
         <v>42</v>
       </c>
       <c r="O6">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P6">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q6">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R6">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S6">
         <v>32</v>
@@ -1249,49 +1258,52 @@
       <c r="AJ6">
         <v>0.75</v>
       </c>
-      <c r="AK6">
-        <v>8</v>
+      <c r="AK6" t="b">
+        <v>0</v>
       </c>
       <c r="AL6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM6">
+        <v>10</v>
+      </c>
+      <c r="AN6">
         <v>-5</v>
       </c>
-      <c r="AN6">
-        <v>1</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>45</v>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:42">
       <c r="A7">
-        <v>21.01098755598068</v>
+        <v>9.700363119443258</v>
       </c>
       <c r="B7">
-        <v>0.2323232323232323</v>
+        <v>0.3737373737373738</v>
       </c>
       <c r="C7">
-        <v>3.85</v>
+        <v>3.67</v>
       </c>
       <c r="D7">
-        <v>17.21</v>
+        <v>6.62</v>
       </c>
       <c r="E7">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F7">
         <v>128</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -1309,16 +1321,16 @@
         <v>42</v>
       </c>
       <c r="O7">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P7">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q7">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R7">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S7">
         <v>32</v>
@@ -1374,49 +1386,52 @@
       <c r="AJ7">
         <v>0.75</v>
       </c>
-      <c r="AK7">
-        <v>8</v>
+      <c r="AK7" t="b">
+        <v>0</v>
       </c>
       <c r="AL7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM7">
+        <v>10</v>
+      </c>
+      <c r="AN7">
         <v>-5</v>
       </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>45</v>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:42">
       <c r="A8">
-        <v>11.10944559176763</v>
+        <v>9.356349666913351</v>
       </c>
       <c r="B8">
-        <v>0.2626262626262627</v>
+        <v>0.3737373737373738</v>
       </c>
       <c r="C8">
-        <v>3.87</v>
+        <v>3.4</v>
       </c>
       <c r="D8">
-        <v>16.46</v>
+        <v>6.62</v>
       </c>
       <c r="E8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F8">
         <v>128</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H8">
         <v>100</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -1431,19 +1446,19 @@
         <v>6</v>
       </c>
       <c r="N8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O8">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P8">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q8">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R8">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S8">
         <v>32</v>
@@ -1499,49 +1514,52 @@
       <c r="AJ8">
         <v>0.75</v>
       </c>
-      <c r="AK8">
-        <v>8</v>
+      <c r="AK8" t="b">
+        <v>0</v>
       </c>
       <c r="AL8">
+        <v>8</v>
+      </c>
+      <c r="AM8">
         <v>5</v>
       </c>
-      <c r="AM8">
-        <v>-5</v>
-      </c>
       <c r="AN8">
-        <v>1</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>45</v>
+        <v>-10</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:42">
       <c r="A9">
-        <v>11.95082873503367</v>
+        <v>9.457663134733837</v>
       </c>
       <c r="B9">
-        <v>0.3434343434343434</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="C9">
-        <v>3.9</v>
+        <v>3.71</v>
       </c>
       <c r="D9">
-        <v>15.49</v>
+        <v>7.08</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F9">
         <v>128</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -1556,19 +1574,19 @@
         <v>6</v>
       </c>
       <c r="N9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O9">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P9">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q9">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R9">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S9">
         <v>32</v>
@@ -1624,49 +1642,52 @@
       <c r="AJ9">
         <v>0.75</v>
       </c>
-      <c r="AK9">
-        <v>8</v>
+      <c r="AK9" t="b">
+        <v>0</v>
       </c>
       <c r="AL9">
+        <v>8</v>
+      </c>
+      <c r="AM9">
         <v>5</v>
       </c>
-      <c r="AM9">
-        <v>-5</v>
-      </c>
       <c r="AN9">
-        <v>1</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>45</v>
+        <v>-10</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:42">
       <c r="A10">
-        <v>11.89163700342178</v>
+        <v>9.457795087496439</v>
       </c>
       <c r="B10">
-        <v>0.4141414141414141</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="C10">
-        <v>3.75</v>
+        <v>3.65</v>
       </c>
       <c r="D10">
-        <v>14.42</v>
+        <v>7.03</v>
       </c>
       <c r="E10">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F10">
         <v>128</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>100</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1681,19 +1702,19 @@
         <v>6</v>
       </c>
       <c r="N10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O10">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P10">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q10">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R10">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S10">
         <v>32</v>
@@ -1749,49 +1770,52 @@
       <c r="AJ10">
         <v>0.75</v>
       </c>
-      <c r="AK10">
-        <v>8</v>
+      <c r="AK10" t="b">
+        <v>0</v>
       </c>
       <c r="AL10">
+        <v>8</v>
+      </c>
+      <c r="AM10">
         <v>5</v>
       </c>
-      <c r="AM10">
-        <v>-5</v>
-      </c>
       <c r="AN10">
-        <v>1</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>45</v>
+        <v>-10</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:42">
       <c r="A11">
-        <v>8.372995054721832</v>
+        <v>9.471425342559815</v>
       </c>
       <c r="B11">
-        <v>0.2424242424242424</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="C11">
-        <v>3.82</v>
+        <v>3.61</v>
       </c>
       <c r="D11">
-        <v>16.87</v>
+        <v>6.77</v>
       </c>
       <c r="E11">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F11">
         <v>128</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H11">
         <v>100</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1806,19 +1830,19 @@
         <v>6</v>
       </c>
       <c r="N11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O11">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P11">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q11">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R11">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S11">
         <v>32</v>
@@ -1874,49 +1898,52 @@
       <c r="AJ11">
         <v>0.75</v>
       </c>
-      <c r="AK11">
-        <v>8</v>
+      <c r="AK11" t="b">
+        <v>0</v>
       </c>
       <c r="AL11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM11">
+        <v>10</v>
+      </c>
+      <c r="AN11">
         <v>-5</v>
       </c>
-      <c r="AN11">
-        <v>1</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>45</v>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:42">
       <c r="A12">
-        <v>8.535145397981008</v>
+        <v>9.724415079752605</v>
       </c>
       <c r="B12">
-        <v>0.1717171717171717</v>
+        <v>0.3434343434343434</v>
       </c>
       <c r="C12">
-        <v>3.91</v>
+        <v>3.58</v>
       </c>
       <c r="D12">
-        <v>17.42</v>
+        <v>6.67</v>
       </c>
       <c r="E12">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F12">
         <v>128</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>100</v>
       </c>
       <c r="I12">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1931,19 +1958,19 @@
         <v>6</v>
       </c>
       <c r="N12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O12">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P12">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q12">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R12">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S12">
         <v>32</v>
@@ -1999,49 +2026,52 @@
       <c r="AJ12">
         <v>0.75</v>
       </c>
-      <c r="AK12">
-        <v>8</v>
+      <c r="AK12" t="b">
+        <v>0</v>
       </c>
       <c r="AL12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM12">
+        <v>10</v>
+      </c>
+      <c r="AN12">
         <v>-5</v>
       </c>
-      <c r="AN12">
-        <v>1</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>45</v>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:42">
       <c r="A13">
-        <v>8.086561504999796</v>
+        <v>9.51093635559082</v>
       </c>
       <c r="B13">
-        <v>0.2323232323232323</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="C13">
-        <v>3.79</v>
+        <v>3.74</v>
       </c>
       <c r="D13">
-        <v>16.81</v>
+        <v>7.35</v>
       </c>
       <c r="E13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F13">
         <v>128</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>100</v>
       </c>
       <c r="I13">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -2056,19 +2086,19 @@
         <v>6</v>
       </c>
       <c r="N13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O13">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="P13">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="Q13">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R13">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="S13">
         <v>32</v>
@@ -2124,20 +2154,2711 @@
       <c r="AJ13">
         <v>0.75</v>
       </c>
-      <c r="AK13">
-        <v>8</v>
+      <c r="AK13" t="b">
+        <v>0</v>
       </c>
       <c r="AL13">
+        <v>8</v>
+      </c>
+      <c r="AM13">
+        <v>10</v>
+      </c>
+      <c r="AN13">
+        <v>-5</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="A14">
+        <v>9.656247814496359</v>
+      </c>
+      <c r="B14">
+        <v>0.2626262626262627</v>
+      </c>
+      <c r="C14">
+        <v>3.66</v>
+      </c>
+      <c r="D14">
+        <v>6.84</v>
+      </c>
+      <c r="E14">
+        <v>500</v>
+      </c>
+      <c r="F14">
+        <v>128</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14">
+        <v>41</v>
+      </c>
+      <c r="P14">
+        <v>215</v>
+      </c>
+      <c r="Q14">
+        <v>42</v>
+      </c>
+      <c r="R14">
+        <v>42</v>
+      </c>
+      <c r="S14">
+        <v>32</v>
+      </c>
+      <c r="T14">
+        <v>32</v>
+      </c>
+      <c r="U14">
+        <v>32</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="X14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>32</v>
+      </c>
+      <c r="Z14">
+        <v>0.9</v>
+      </c>
+      <c r="AA14">
+        <v>0.01</v>
+      </c>
+      <c r="AB14">
+        <v>32</v>
+      </c>
+      <c r="AC14">
+        <v>10</v>
+      </c>
+      <c r="AD14">
+        <v>0.3</v>
+      </c>
+      <c r="AE14">
+        <v>0.95</v>
+      </c>
+      <c r="AF14">
+        <v>0.001</v>
+      </c>
+      <c r="AG14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <v>0.75</v>
+      </c>
+      <c r="AK14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>8</v>
+      </c>
+      <c r="AM14">
+        <v>2</v>
+      </c>
+      <c r="AN14">
+        <v>-2</v>
+      </c>
+      <c r="AO14">
+        <v>1</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="A15">
+        <v>9.345927798748017</v>
+      </c>
+      <c r="B15">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="C15">
+        <v>3.59</v>
+      </c>
+      <c r="D15">
+        <v>7.14</v>
+      </c>
+      <c r="E15">
+        <v>500</v>
+      </c>
+      <c r="F15">
+        <v>128</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15">
+        <v>41</v>
+      </c>
+      <c r="P15">
+        <v>215</v>
+      </c>
+      <c r="Q15">
+        <v>42</v>
+      </c>
+      <c r="R15">
+        <v>42</v>
+      </c>
+      <c r="S15">
+        <v>32</v>
+      </c>
+      <c r="T15">
+        <v>32</v>
+      </c>
+      <c r="U15">
+        <v>32</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>2</v>
+      </c>
+      <c r="X15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>32</v>
+      </c>
+      <c r="Z15">
+        <v>0.9</v>
+      </c>
+      <c r="AA15">
+        <v>0.01</v>
+      </c>
+      <c r="AB15">
+        <v>32</v>
+      </c>
+      <c r="AC15">
+        <v>10</v>
+      </c>
+      <c r="AD15">
+        <v>0.3</v>
+      </c>
+      <c r="AE15">
+        <v>0.95</v>
+      </c>
+      <c r="AF15">
+        <v>0.001</v>
+      </c>
+      <c r="AG15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15">
+        <v>0.75</v>
+      </c>
+      <c r="AK15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>8</v>
+      </c>
+      <c r="AM15">
+        <v>2</v>
+      </c>
+      <c r="AN15">
+        <v>-2</v>
+      </c>
+      <c r="AO15">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="A16">
+        <v>9.439344414075215</v>
+      </c>
+      <c r="B16">
+        <v>0.3131313131313131</v>
+      </c>
+      <c r="C16">
+        <v>3.52</v>
+      </c>
+      <c r="D16">
+        <v>6.82</v>
+      </c>
+      <c r="E16">
+        <v>500</v>
+      </c>
+      <c r="F16">
+        <v>128</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16">
+        <v>41</v>
+      </c>
+      <c r="P16">
+        <v>215</v>
+      </c>
+      <c r="Q16">
+        <v>42</v>
+      </c>
+      <c r="R16">
+        <v>42</v>
+      </c>
+      <c r="S16">
+        <v>32</v>
+      </c>
+      <c r="T16">
+        <v>32</v>
+      </c>
+      <c r="U16">
+        <v>32</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+      <c r="X16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>32</v>
+      </c>
+      <c r="Z16">
+        <v>0.9</v>
+      </c>
+      <c r="AA16">
+        <v>0.01</v>
+      </c>
+      <c r="AB16">
+        <v>32</v>
+      </c>
+      <c r="AC16">
+        <v>10</v>
+      </c>
+      <c r="AD16">
+        <v>0.3</v>
+      </c>
+      <c r="AE16">
+        <v>0.95</v>
+      </c>
+      <c r="AF16">
+        <v>0.001</v>
+      </c>
+      <c r="AG16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
+        <v>0.75</v>
+      </c>
+      <c r="AK16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>8</v>
+      </c>
+      <c r="AM16">
+        <v>2</v>
+      </c>
+      <c r="AN16">
+        <v>-2</v>
+      </c>
+      <c r="AO16">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42">
+      <c r="A17">
+        <v>9.553007423877716</v>
+      </c>
+      <c r="B17">
+        <v>0.3232323232323233</v>
+      </c>
+      <c r="C17">
+        <v>3.64</v>
+      </c>
+      <c r="D17">
+        <v>6.94</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+      <c r="F17">
+        <v>128</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>6</v>
+      </c>
+      <c r="N17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17">
+        <v>41</v>
+      </c>
+      <c r="P17">
+        <v>215</v>
+      </c>
+      <c r="Q17">
+        <v>42</v>
+      </c>
+      <c r="R17">
+        <v>42</v>
+      </c>
+      <c r="S17">
+        <v>32</v>
+      </c>
+      <c r="T17">
+        <v>32</v>
+      </c>
+      <c r="U17">
+        <v>32</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>2</v>
+      </c>
+      <c r="X17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <v>32</v>
+      </c>
+      <c r="Z17">
+        <v>0.9</v>
+      </c>
+      <c r="AA17">
+        <v>0.01</v>
+      </c>
+      <c r="AB17">
+        <v>32</v>
+      </c>
+      <c r="AC17">
+        <v>10</v>
+      </c>
+      <c r="AD17">
+        <v>0.3</v>
+      </c>
+      <c r="AE17">
+        <v>0.95</v>
+      </c>
+      <c r="AF17">
+        <v>0.001</v>
+      </c>
+      <c r="AG17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
+        <v>1</v>
+      </c>
+      <c r="AJ17">
+        <v>0.75</v>
+      </c>
+      <c r="AK17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>8</v>
+      </c>
+      <c r="AM17">
+        <v>10</v>
+      </c>
+      <c r="AN17">
+        <v>-2</v>
+      </c>
+      <c r="AO17">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42">
+      <c r="A18">
+        <v>9.764042945702871</v>
+      </c>
+      <c r="B18">
+        <v>0.2626262626262627</v>
+      </c>
+      <c r="C18">
+        <v>3.58</v>
+      </c>
+      <c r="D18">
+        <v>7.03</v>
+      </c>
+      <c r="E18">
+        <v>500</v>
+      </c>
+      <c r="F18">
+        <v>128</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+      <c r="N18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18">
+        <v>41</v>
+      </c>
+      <c r="P18">
+        <v>215</v>
+      </c>
+      <c r="Q18">
+        <v>42</v>
+      </c>
+      <c r="R18">
+        <v>42</v>
+      </c>
+      <c r="S18">
+        <v>32</v>
+      </c>
+      <c r="T18">
+        <v>32</v>
+      </c>
+      <c r="U18">
+        <v>32</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>2</v>
+      </c>
+      <c r="X18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>32</v>
+      </c>
+      <c r="Z18">
+        <v>0.9</v>
+      </c>
+      <c r="AA18">
+        <v>0.01</v>
+      </c>
+      <c r="AB18">
+        <v>32</v>
+      </c>
+      <c r="AC18">
+        <v>10</v>
+      </c>
+      <c r="AD18">
+        <v>0.3</v>
+      </c>
+      <c r="AE18">
+        <v>0.95</v>
+      </c>
+      <c r="AF18">
+        <v>0.001</v>
+      </c>
+      <c r="AG18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>0.75</v>
+      </c>
+      <c r="AK18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>8</v>
+      </c>
+      <c r="AM18">
+        <v>10</v>
+      </c>
+      <c r="AN18">
+        <v>-2</v>
+      </c>
+      <c r="AO18">
+        <v>1</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42">
+      <c r="A19">
+        <v>9.728737215201059</v>
+      </c>
+      <c r="B19">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="C19">
+        <v>3.63</v>
+      </c>
+      <c r="D19">
+        <v>6.9</v>
+      </c>
+      <c r="E19">
+        <v>500</v>
+      </c>
+      <c r="F19">
+        <v>128</v>
+      </c>
+      <c r="G19">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>6</v>
+      </c>
+      <c r="N19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O19">
+        <v>41</v>
+      </c>
+      <c r="P19">
+        <v>215</v>
+      </c>
+      <c r="Q19">
+        <v>42</v>
+      </c>
+      <c r="R19">
+        <v>42</v>
+      </c>
+      <c r="S19">
+        <v>32</v>
+      </c>
+      <c r="T19">
+        <v>32</v>
+      </c>
+      <c r="U19">
+        <v>32</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>2</v>
+      </c>
+      <c r="X19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>32</v>
+      </c>
+      <c r="Z19">
+        <v>0.9</v>
+      </c>
+      <c r="AA19">
+        <v>0.01</v>
+      </c>
+      <c r="AB19">
+        <v>32</v>
+      </c>
+      <c r="AC19">
+        <v>10</v>
+      </c>
+      <c r="AD19">
+        <v>0.3</v>
+      </c>
+      <c r="AE19">
+        <v>0.95</v>
+      </c>
+      <c r="AF19">
+        <v>0.001</v>
+      </c>
+      <c r="AG19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>0.75</v>
+      </c>
+      <c r="AK19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>8</v>
+      </c>
+      <c r="AM19">
+        <v>10</v>
+      </c>
+      <c r="AN19">
+        <v>-2</v>
+      </c>
+      <c r="AO19">
+        <v>1</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
+      <c r="A20">
+        <v>9.822686127821605</v>
+      </c>
+      <c r="B20">
+        <v>0.2626262626262627</v>
+      </c>
+      <c r="C20">
+        <v>3.54</v>
+      </c>
+      <c r="D20">
+        <v>7.11</v>
+      </c>
+      <c r="E20">
+        <v>500</v>
+      </c>
+      <c r="F20">
+        <v>128</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20">
+        <v>41</v>
+      </c>
+      <c r="P20">
+        <v>215</v>
+      </c>
+      <c r="Q20">
+        <v>42</v>
+      </c>
+      <c r="R20">
+        <v>42</v>
+      </c>
+      <c r="S20">
+        <v>32</v>
+      </c>
+      <c r="T20">
+        <v>32</v>
+      </c>
+      <c r="U20">
+        <v>32</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>2</v>
+      </c>
+      <c r="X20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>32</v>
+      </c>
+      <c r="Z20">
+        <v>0.9</v>
+      </c>
+      <c r="AA20">
+        <v>0.01</v>
+      </c>
+      <c r="AB20">
+        <v>32</v>
+      </c>
+      <c r="AC20">
+        <v>10</v>
+      </c>
+      <c r="AD20">
+        <v>0.3</v>
+      </c>
+      <c r="AE20">
+        <v>0.95</v>
+      </c>
+      <c r="AF20">
+        <v>0.001</v>
+      </c>
+      <c r="AG20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
+        <v>1</v>
+      </c>
+      <c r="AJ20">
+        <v>0.75</v>
+      </c>
+      <c r="AK20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>8</v>
+      </c>
+      <c r="AM20">
+        <v>2</v>
+      </c>
+      <c r="AN20">
+        <v>-10</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42">
+      <c r="A21">
+        <v>10.11651712656021</v>
+      </c>
+      <c r="B21">
+        <v>0.3434343434343434</v>
+      </c>
+      <c r="C21">
+        <v>3.52</v>
+      </c>
+      <c r="D21">
+        <v>6.82</v>
+      </c>
+      <c r="E21">
+        <v>500</v>
+      </c>
+      <c r="F21">
+        <v>128</v>
+      </c>
+      <c r="G21">
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>42</v>
+      </c>
+      <c r="O21">
+        <v>41</v>
+      </c>
+      <c r="P21">
+        <v>215</v>
+      </c>
+      <c r="Q21">
+        <v>42</v>
+      </c>
+      <c r="R21">
+        <v>42</v>
+      </c>
+      <c r="S21">
+        <v>32</v>
+      </c>
+      <c r="T21">
+        <v>32</v>
+      </c>
+      <c r="U21">
+        <v>32</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>2</v>
+      </c>
+      <c r="X21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>32</v>
+      </c>
+      <c r="Z21">
+        <v>0.9</v>
+      </c>
+      <c r="AA21">
+        <v>0.01</v>
+      </c>
+      <c r="AB21">
+        <v>32</v>
+      </c>
+      <c r="AC21">
+        <v>10</v>
+      </c>
+      <c r="AD21">
+        <v>0.3</v>
+      </c>
+      <c r="AE21">
+        <v>0.95</v>
+      </c>
+      <c r="AF21">
+        <v>0.001</v>
+      </c>
+      <c r="AG21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>0.75</v>
+      </c>
+      <c r="AK21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>8</v>
+      </c>
+      <c r="AM21">
+        <v>2</v>
+      </c>
+      <c r="AN21">
+        <v>-10</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42">
+      <c r="A22">
+        <v>9.545294499397277</v>
+      </c>
+      <c r="B22">
+        <v>0.3232323232323233</v>
+      </c>
+      <c r="C22">
+        <v>3.66</v>
+      </c>
+      <c r="D22">
+        <v>6.92</v>
+      </c>
+      <c r="E22">
+        <v>500</v>
+      </c>
+      <c r="F22">
+        <v>128</v>
+      </c>
+      <c r="G22">
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22" t="s">
+        <v>42</v>
+      </c>
+      <c r="O22">
+        <v>41</v>
+      </c>
+      <c r="P22">
+        <v>215</v>
+      </c>
+      <c r="Q22">
+        <v>42</v>
+      </c>
+      <c r="R22">
+        <v>42</v>
+      </c>
+      <c r="S22">
+        <v>32</v>
+      </c>
+      <c r="T22">
+        <v>32</v>
+      </c>
+      <c r="U22">
+        <v>32</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>2</v>
+      </c>
+      <c r="X22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>32</v>
+      </c>
+      <c r="Z22">
+        <v>0.9</v>
+      </c>
+      <c r="AA22">
+        <v>0.01</v>
+      </c>
+      <c r="AB22">
+        <v>32</v>
+      </c>
+      <c r="AC22">
+        <v>10</v>
+      </c>
+      <c r="AD22">
+        <v>0.3</v>
+      </c>
+      <c r="AE22">
+        <v>0.95</v>
+      </c>
+      <c r="AF22">
+        <v>0.001</v>
+      </c>
+      <c r="AG22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>0.75</v>
+      </c>
+      <c r="AK22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>8</v>
+      </c>
+      <c r="AM22">
+        <v>2</v>
+      </c>
+      <c r="AN22">
+        <v>-10</v>
+      </c>
+      <c r="AO22">
+        <v>1</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42">
+      <c r="A23">
+        <v>9.587398576736451</v>
+      </c>
+      <c r="B23">
+        <v>0.3232323232323233</v>
+      </c>
+      <c r="C23">
+        <v>3.63</v>
+      </c>
+      <c r="D23">
+        <v>7.07</v>
+      </c>
+      <c r="E23">
+        <v>500</v>
+      </c>
+      <c r="F23">
+        <v>128</v>
+      </c>
+      <c r="G23">
+        <v>50</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
+        <v>6</v>
+      </c>
+      <c r="N23" t="s">
+        <v>42</v>
+      </c>
+      <c r="O23">
+        <v>41</v>
+      </c>
+      <c r="P23">
+        <v>215</v>
+      </c>
+      <c r="Q23">
+        <v>42</v>
+      </c>
+      <c r="R23">
+        <v>42</v>
+      </c>
+      <c r="S23">
+        <v>32</v>
+      </c>
+      <c r="T23">
+        <v>32</v>
+      </c>
+      <c r="U23">
+        <v>32</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="X23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>32</v>
+      </c>
+      <c r="Z23">
+        <v>0.9</v>
+      </c>
+      <c r="AA23">
+        <v>0.01</v>
+      </c>
+      <c r="AB23">
+        <v>32</v>
+      </c>
+      <c r="AC23">
+        <v>10</v>
+      </c>
+      <c r="AD23">
+        <v>0.3</v>
+      </c>
+      <c r="AE23">
+        <v>0.95</v>
+      </c>
+      <c r="AF23">
+        <v>0.001</v>
+      </c>
+      <c r="AG23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
+      </c>
+      <c r="AI23">
+        <v>1</v>
+      </c>
+      <c r="AJ23">
+        <v>0.75</v>
+      </c>
+      <c r="AK23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>8</v>
+      </c>
+      <c r="AM23">
+        <v>10</v>
+      </c>
+      <c r="AN23">
+        <v>-2</v>
+      </c>
+      <c r="AO23">
+        <v>1</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42">
+      <c r="A24">
+        <v>9.508966739972433</v>
+      </c>
+      <c r="B24">
+        <v>0.404040404040404</v>
+      </c>
+      <c r="C24">
+        <v>3.51</v>
+      </c>
+      <c r="D24">
+        <v>6.86</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
+      <c r="F24">
+        <v>128</v>
+      </c>
+      <c r="G24">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <v>8</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>6</v>
+      </c>
+      <c r="N24" t="s">
+        <v>42</v>
+      </c>
+      <c r="O24">
+        <v>41</v>
+      </c>
+      <c r="P24">
+        <v>215</v>
+      </c>
+      <c r="Q24">
+        <v>42</v>
+      </c>
+      <c r="R24">
+        <v>42</v>
+      </c>
+      <c r="S24">
+        <v>32</v>
+      </c>
+      <c r="T24">
+        <v>32</v>
+      </c>
+      <c r="U24">
+        <v>32</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>2</v>
+      </c>
+      <c r="X24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>32</v>
+      </c>
+      <c r="Z24">
+        <v>0.9</v>
+      </c>
+      <c r="AA24">
+        <v>0.01</v>
+      </c>
+      <c r="AB24">
+        <v>32</v>
+      </c>
+      <c r="AC24">
+        <v>10</v>
+      </c>
+      <c r="AD24">
+        <v>0.3</v>
+      </c>
+      <c r="AE24">
+        <v>0.95</v>
+      </c>
+      <c r="AF24">
+        <v>0.001</v>
+      </c>
+      <c r="AG24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
+      <c r="AI24">
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <v>0.75</v>
+      </c>
+      <c r="AK24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>8</v>
+      </c>
+      <c r="AM24">
+        <v>10</v>
+      </c>
+      <c r="AN24">
+        <v>-2</v>
+      </c>
+      <c r="AO24">
+        <v>1</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42">
+      <c r="A25">
+        <v>9.802822570006052</v>
+      </c>
+      <c r="B25">
+        <v>0.2828282828282828</v>
+      </c>
+      <c r="C25">
+        <v>3.73</v>
+      </c>
+      <c r="D25">
+        <v>6.84</v>
+      </c>
+      <c r="E25">
+        <v>500</v>
+      </c>
+      <c r="F25">
+        <v>128</v>
+      </c>
+      <c r="G25">
+        <v>50</v>
+      </c>
+      <c r="H25">
+        <v>100</v>
+      </c>
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>6</v>
+      </c>
+      <c r="N25" t="s">
+        <v>42</v>
+      </c>
+      <c r="O25">
+        <v>41</v>
+      </c>
+      <c r="P25">
+        <v>215</v>
+      </c>
+      <c r="Q25">
+        <v>42</v>
+      </c>
+      <c r="R25">
+        <v>42</v>
+      </c>
+      <c r="S25">
+        <v>32</v>
+      </c>
+      <c r="T25">
+        <v>32</v>
+      </c>
+      <c r="U25">
+        <v>32</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>2</v>
+      </c>
+      <c r="X25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>32</v>
+      </c>
+      <c r="Z25">
+        <v>0.9</v>
+      </c>
+      <c r="AA25">
+        <v>0.01</v>
+      </c>
+      <c r="AB25">
+        <v>32</v>
+      </c>
+      <c r="AC25">
+        <v>10</v>
+      </c>
+      <c r="AD25">
+        <v>0.3</v>
+      </c>
+      <c r="AE25">
+        <v>0.95</v>
+      </c>
+      <c r="AF25">
+        <v>0.001</v>
+      </c>
+      <c r="AG25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>1</v>
+      </c>
+      <c r="AI25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>0.75</v>
+      </c>
+      <c r="AK25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>8</v>
+      </c>
+      <c r="AM25">
+        <v>10</v>
+      </c>
+      <c r="AN25">
+        <v>-2</v>
+      </c>
+      <c r="AO25">
+        <v>1</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42">
+      <c r="A26">
+        <v>9.647055713335673</v>
+      </c>
+      <c r="B26">
+        <v>0.2525252525252525</v>
+      </c>
+      <c r="C26">
+        <v>3.58</v>
+      </c>
+      <c r="D26">
+        <v>6.88</v>
+      </c>
+      <c r="E26">
+        <v>500</v>
+      </c>
+      <c r="F26">
+        <v>128</v>
+      </c>
+      <c r="G26">
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26">
+        <v>6</v>
+      </c>
+      <c r="N26" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26">
+        <v>41</v>
+      </c>
+      <c r="P26">
+        <v>215</v>
+      </c>
+      <c r="Q26">
+        <v>42</v>
+      </c>
+      <c r="R26">
+        <v>42</v>
+      </c>
+      <c r="S26">
+        <v>32</v>
+      </c>
+      <c r="T26">
+        <v>32</v>
+      </c>
+      <c r="U26">
+        <v>32</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>2</v>
+      </c>
+      <c r="X26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>32</v>
+      </c>
+      <c r="Z26">
+        <v>0.9</v>
+      </c>
+      <c r="AA26">
+        <v>0.01</v>
+      </c>
+      <c r="AB26">
+        <v>32</v>
+      </c>
+      <c r="AC26">
+        <v>10</v>
+      </c>
+      <c r="AD26">
+        <v>0.3</v>
+      </c>
+      <c r="AE26">
+        <v>0.95</v>
+      </c>
+      <c r="AF26">
+        <v>0.001</v>
+      </c>
+      <c r="AG26" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH26">
+        <v>1</v>
+      </c>
+      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AJ26">
+        <v>0.75</v>
+      </c>
+      <c r="AK26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>8</v>
+      </c>
+      <c r="AM26">
         <v>5</v>
       </c>
-      <c r="AM13">
+      <c r="AN26">
         <v>-5</v>
       </c>
-      <c r="AN13">
-        <v>1</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>45</v>
+      <c r="AO26">
+        <v>1</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42">
+      <c r="A27">
+        <v>9.746423387527466</v>
+      </c>
+      <c r="B27">
+        <v>0.3131313131313131</v>
+      </c>
+      <c r="C27">
+        <v>3.62</v>
+      </c>
+      <c r="D27">
+        <v>6.82</v>
+      </c>
+      <c r="E27">
+        <v>500</v>
+      </c>
+      <c r="F27">
+        <v>128</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>6</v>
+      </c>
+      <c r="N27" t="s">
+        <v>42</v>
+      </c>
+      <c r="O27">
+        <v>41</v>
+      </c>
+      <c r="P27">
+        <v>215</v>
+      </c>
+      <c r="Q27">
+        <v>42</v>
+      </c>
+      <c r="R27">
+        <v>42</v>
+      </c>
+      <c r="S27">
+        <v>32</v>
+      </c>
+      <c r="T27">
+        <v>32</v>
+      </c>
+      <c r="U27">
+        <v>32</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>2</v>
+      </c>
+      <c r="X27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>32</v>
+      </c>
+      <c r="Z27">
+        <v>0.9</v>
+      </c>
+      <c r="AA27">
+        <v>0.01</v>
+      </c>
+      <c r="AB27">
+        <v>32</v>
+      </c>
+      <c r="AC27">
+        <v>10</v>
+      </c>
+      <c r="AD27">
+        <v>0.3</v>
+      </c>
+      <c r="AE27">
+        <v>0.95</v>
+      </c>
+      <c r="AF27">
+        <v>0.001</v>
+      </c>
+      <c r="AG27" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
+        <v>1</v>
+      </c>
+      <c r="AJ27">
+        <v>0.75</v>
+      </c>
+      <c r="AK27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>8</v>
+      </c>
+      <c r="AM27">
+        <v>5</v>
+      </c>
+      <c r="AN27">
+        <v>-5</v>
+      </c>
+      <c r="AO27">
+        <v>1</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42">
+      <c r="A28">
+        <v>9.620925601323446</v>
+      </c>
+      <c r="B28">
+        <v>0.4141414141414141</v>
+      </c>
+      <c r="C28">
+        <v>3.61</v>
+      </c>
+      <c r="D28">
+        <v>6.7</v>
+      </c>
+      <c r="E28">
+        <v>500</v>
+      </c>
+      <c r="F28">
+        <v>128</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>6</v>
+      </c>
+      <c r="N28" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28">
+        <v>41</v>
+      </c>
+      <c r="P28">
+        <v>215</v>
+      </c>
+      <c r="Q28">
+        <v>42</v>
+      </c>
+      <c r="R28">
+        <v>42</v>
+      </c>
+      <c r="S28">
+        <v>32</v>
+      </c>
+      <c r="T28">
+        <v>32</v>
+      </c>
+      <c r="U28">
+        <v>32</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>2</v>
+      </c>
+      <c r="X28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>32</v>
+      </c>
+      <c r="Z28">
+        <v>0.9</v>
+      </c>
+      <c r="AA28">
+        <v>0.01</v>
+      </c>
+      <c r="AB28">
+        <v>32</v>
+      </c>
+      <c r="AC28">
+        <v>10</v>
+      </c>
+      <c r="AD28">
+        <v>0.3</v>
+      </c>
+      <c r="AE28">
+        <v>0.95</v>
+      </c>
+      <c r="AF28">
+        <v>0.001</v>
+      </c>
+      <c r="AG28" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
+        <v>1</v>
+      </c>
+      <c r="AJ28">
+        <v>0.75</v>
+      </c>
+      <c r="AK28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>8</v>
+      </c>
+      <c r="AM28">
+        <v>5</v>
+      </c>
+      <c r="AN28">
+        <v>-5</v>
+      </c>
+      <c r="AO28">
+        <v>1</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42">
+      <c r="A29">
+        <v>9.688162469863892</v>
+      </c>
+      <c r="B29">
+        <v>0.2828282828282828</v>
+      </c>
+      <c r="C29">
+        <v>3.67</v>
+      </c>
+      <c r="D29">
+        <v>7.03</v>
+      </c>
+      <c r="E29">
+        <v>500</v>
+      </c>
+      <c r="F29">
+        <v>128</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>100</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <v>6</v>
+      </c>
+      <c r="N29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O29">
+        <v>41</v>
+      </c>
+      <c r="P29">
+        <v>215</v>
+      </c>
+      <c r="Q29">
+        <v>42</v>
+      </c>
+      <c r="R29">
+        <v>42</v>
+      </c>
+      <c r="S29">
+        <v>32</v>
+      </c>
+      <c r="T29">
+        <v>32</v>
+      </c>
+      <c r="U29">
+        <v>32</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>2</v>
+      </c>
+      <c r="X29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>32</v>
+      </c>
+      <c r="Z29">
+        <v>0.9</v>
+      </c>
+      <c r="AA29">
+        <v>0.01</v>
+      </c>
+      <c r="AB29">
+        <v>32</v>
+      </c>
+      <c r="AC29">
+        <v>10</v>
+      </c>
+      <c r="AD29">
+        <v>0.3</v>
+      </c>
+      <c r="AE29">
+        <v>0.95</v>
+      </c>
+      <c r="AF29">
+        <v>0.001</v>
+      </c>
+      <c r="AG29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>1</v>
+      </c>
+      <c r="AJ29">
+        <v>0.75</v>
+      </c>
+      <c r="AK29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <v>8</v>
+      </c>
+      <c r="AM29">
+        <v>5</v>
+      </c>
+      <c r="AN29">
+        <v>-2</v>
+      </c>
+      <c r="AO29">
+        <v>1</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42">
+      <c r="A30">
+        <v>9.384997701644897</v>
+      </c>
+      <c r="B30">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="C30">
+        <v>3.67</v>
+      </c>
+      <c r="D30">
+        <v>6.96</v>
+      </c>
+      <c r="E30">
+        <v>500</v>
+      </c>
+      <c r="F30">
+        <v>128</v>
+      </c>
+      <c r="G30">
+        <v>50</v>
+      </c>
+      <c r="H30">
+        <v>100</v>
+      </c>
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <v>6</v>
+      </c>
+      <c r="N30" t="s">
+        <v>42</v>
+      </c>
+      <c r="O30">
+        <v>41</v>
+      </c>
+      <c r="P30">
+        <v>215</v>
+      </c>
+      <c r="Q30">
+        <v>42</v>
+      </c>
+      <c r="R30">
+        <v>42</v>
+      </c>
+      <c r="S30">
+        <v>32</v>
+      </c>
+      <c r="T30">
+        <v>32</v>
+      </c>
+      <c r="U30">
+        <v>32</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
+      </c>
+      <c r="X30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>32</v>
+      </c>
+      <c r="Z30">
+        <v>0.9</v>
+      </c>
+      <c r="AA30">
+        <v>0.01</v>
+      </c>
+      <c r="AB30">
+        <v>32</v>
+      </c>
+      <c r="AC30">
+        <v>10</v>
+      </c>
+      <c r="AD30">
+        <v>0.3</v>
+      </c>
+      <c r="AE30">
+        <v>0.95</v>
+      </c>
+      <c r="AF30">
+        <v>0.001</v>
+      </c>
+      <c r="AG30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH30">
+        <v>1</v>
+      </c>
+      <c r="AI30">
+        <v>1</v>
+      </c>
+      <c r="AJ30">
+        <v>0.75</v>
+      </c>
+      <c r="AK30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>8</v>
+      </c>
+      <c r="AM30">
+        <v>5</v>
+      </c>
+      <c r="AN30">
+        <v>-2</v>
+      </c>
+      <c r="AO30">
+        <v>1</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42">
+      <c r="A31">
+        <v>9.702756790320079</v>
+      </c>
+      <c r="B31">
+        <v>0.3232323232323233</v>
+      </c>
+      <c r="C31">
+        <v>3.55</v>
+      </c>
+      <c r="D31">
+        <v>6.83</v>
+      </c>
+      <c r="E31">
+        <v>500</v>
+      </c>
+      <c r="F31">
+        <v>128</v>
+      </c>
+      <c r="G31">
+        <v>50</v>
+      </c>
+      <c r="H31">
+        <v>100</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="M31">
+        <v>6</v>
+      </c>
+      <c r="N31" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31">
+        <v>41</v>
+      </c>
+      <c r="P31">
+        <v>215</v>
+      </c>
+      <c r="Q31">
+        <v>42</v>
+      </c>
+      <c r="R31">
+        <v>42</v>
+      </c>
+      <c r="S31">
+        <v>32</v>
+      </c>
+      <c r="T31">
+        <v>32</v>
+      </c>
+      <c r="U31">
+        <v>32</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>2</v>
+      </c>
+      <c r="X31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <v>32</v>
+      </c>
+      <c r="Z31">
+        <v>0.9</v>
+      </c>
+      <c r="AA31">
+        <v>0.01</v>
+      </c>
+      <c r="AB31">
+        <v>32</v>
+      </c>
+      <c r="AC31">
+        <v>10</v>
+      </c>
+      <c r="AD31">
+        <v>0.3</v>
+      </c>
+      <c r="AE31">
+        <v>0.95</v>
+      </c>
+      <c r="AF31">
+        <v>0.001</v>
+      </c>
+      <c r="AG31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH31">
+        <v>1</v>
+      </c>
+      <c r="AI31">
+        <v>1</v>
+      </c>
+      <c r="AJ31">
+        <v>0.75</v>
+      </c>
+      <c r="AK31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>8</v>
+      </c>
+      <c r="AM31">
+        <v>5</v>
+      </c>
+      <c r="AN31">
+        <v>-2</v>
+      </c>
+      <c r="AO31">
+        <v>1</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42">
+      <c r="A32">
+        <v>9.035989149411519</v>
+      </c>
+      <c r="B32">
+        <v>0.2929292929292929</v>
+      </c>
+      <c r="C32">
+        <v>3.56</v>
+      </c>
+      <c r="D32">
+        <v>6.91</v>
+      </c>
+      <c r="E32">
+        <v>500</v>
+      </c>
+      <c r="F32">
+        <v>128</v>
+      </c>
+      <c r="G32">
+        <v>50</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32" t="s">
+        <v>42</v>
+      </c>
+      <c r="O32">
+        <v>41</v>
+      </c>
+      <c r="P32">
+        <v>215</v>
+      </c>
+      <c r="Q32">
+        <v>42</v>
+      </c>
+      <c r="R32">
+        <v>42</v>
+      </c>
+      <c r="S32">
+        <v>32</v>
+      </c>
+      <c r="T32">
+        <v>32</v>
+      </c>
+      <c r="U32">
+        <v>32</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>2</v>
+      </c>
+      <c r="X32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <v>32</v>
+      </c>
+      <c r="Z32">
+        <v>0.9</v>
+      </c>
+      <c r="AA32">
+        <v>0.01</v>
+      </c>
+      <c r="AB32">
+        <v>32</v>
+      </c>
+      <c r="AC32">
+        <v>10</v>
+      </c>
+      <c r="AD32">
+        <v>0.3</v>
+      </c>
+      <c r="AE32">
+        <v>0.95</v>
+      </c>
+      <c r="AF32">
+        <v>0.001</v>
+      </c>
+      <c r="AG32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH32">
+        <v>1</v>
+      </c>
+      <c r="AI32">
+        <v>1</v>
+      </c>
+      <c r="AJ32">
+        <v>0.75</v>
+      </c>
+      <c r="AK32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>8</v>
+      </c>
+      <c r="AM32">
+        <v>2</v>
+      </c>
+      <c r="AN32">
+        <v>-10</v>
+      </c>
+      <c r="AO32">
+        <v>1</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42">
+      <c r="A33">
+        <v>9.421159732341767</v>
+      </c>
+      <c r="B33">
+        <v>0.2929292929292929</v>
+      </c>
+      <c r="C33">
+        <v>3.61</v>
+      </c>
+      <c r="D33">
+        <v>6.75</v>
+      </c>
+      <c r="E33">
+        <v>500</v>
+      </c>
+      <c r="F33">
+        <v>128</v>
+      </c>
+      <c r="G33">
+        <v>50</v>
+      </c>
+      <c r="H33">
+        <v>100</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>6</v>
+      </c>
+      <c r="N33" t="s">
+        <v>42</v>
+      </c>
+      <c r="O33">
+        <v>41</v>
+      </c>
+      <c r="P33">
+        <v>215</v>
+      </c>
+      <c r="Q33">
+        <v>42</v>
+      </c>
+      <c r="R33">
+        <v>42</v>
+      </c>
+      <c r="S33">
+        <v>32</v>
+      </c>
+      <c r="T33">
+        <v>32</v>
+      </c>
+      <c r="U33">
+        <v>32</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>2</v>
+      </c>
+      <c r="X33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <v>32</v>
+      </c>
+      <c r="Z33">
+        <v>0.9</v>
+      </c>
+      <c r="AA33">
+        <v>0.01</v>
+      </c>
+      <c r="AB33">
+        <v>32</v>
+      </c>
+      <c r="AC33">
+        <v>10</v>
+      </c>
+      <c r="AD33">
+        <v>0.3</v>
+      </c>
+      <c r="AE33">
+        <v>0.95</v>
+      </c>
+      <c r="AF33">
+        <v>0.001</v>
+      </c>
+      <c r="AG33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH33">
+        <v>1</v>
+      </c>
+      <c r="AI33">
+        <v>1</v>
+      </c>
+      <c r="AJ33">
+        <v>0.75</v>
+      </c>
+      <c r="AK33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>8</v>
+      </c>
+      <c r="AM33">
+        <v>2</v>
+      </c>
+      <c r="AN33">
+        <v>-10</v>
+      </c>
+      <c r="AO33">
+        <v>1</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42">
+      <c r="A34">
+        <v>8.906918287277222</v>
+      </c>
+      <c r="B34">
+        <v>0.2626262626262627</v>
+      </c>
+      <c r="C34">
+        <v>3.67</v>
+      </c>
+      <c r="D34">
+        <v>6.86</v>
+      </c>
+      <c r="E34">
+        <v>500</v>
+      </c>
+      <c r="F34">
+        <v>128</v>
+      </c>
+      <c r="G34">
+        <v>50</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+      <c r="I34">
+        <v>8</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>6</v>
+      </c>
+      <c r="N34" t="s">
+        <v>42</v>
+      </c>
+      <c r="O34">
+        <v>41</v>
+      </c>
+      <c r="P34">
+        <v>215</v>
+      </c>
+      <c r="Q34">
+        <v>42</v>
+      </c>
+      <c r="R34">
+        <v>42</v>
+      </c>
+      <c r="S34">
+        <v>32</v>
+      </c>
+      <c r="T34">
+        <v>32</v>
+      </c>
+      <c r="U34">
+        <v>32</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>2</v>
+      </c>
+      <c r="X34" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>32</v>
+      </c>
+      <c r="Z34">
+        <v>0.9</v>
+      </c>
+      <c r="AA34">
+        <v>0.01</v>
+      </c>
+      <c r="AB34">
+        <v>32</v>
+      </c>
+      <c r="AC34">
+        <v>10</v>
+      </c>
+      <c r="AD34">
+        <v>0.3</v>
+      </c>
+      <c r="AE34">
+        <v>0.95</v>
+      </c>
+      <c r="AF34">
+        <v>0.001</v>
+      </c>
+      <c r="AG34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH34">
+        <v>1</v>
+      </c>
+      <c r="AI34">
+        <v>1</v>
+      </c>
+      <c r="AJ34">
+        <v>0.75</v>
+      </c>
+      <c r="AK34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>8</v>
+      </c>
+      <c r="AM34">
+        <v>2</v>
+      </c>
+      <c r="AN34">
+        <v>-10</v>
+      </c>
+      <c r="AO34">
+        <v>1</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>